<commit_message>
Document hypothesis and related strategies grouped into 3 areas - Personal development, Professional development and Work life balance. Started codiying and implemented phase 1 of the recommendation algorithm for personal development strategies.
</commit_message>
<xml_diff>
--- a/05_evaluation/recommendation_strategy_development_sheet.xlsx
+++ b/05_evaluation/recommendation_strategy_development_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdanc\Desktop\HR_201_Employee_Attrition_Project\06_Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/695975/Documents/DataScience/business-science/HR201_employee_attrition/05_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8BFAADD7-5517-414A-B370-CD3FB25C09FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363B9C26-78A2-0F41-8712-E653B7DF57C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy Worksheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>Feature</t>
   </si>
@@ -142,12 +142,138 @@
   <si>
     <t xml:space="preserve"> Used to investigate the relationship between values within features and the target (Attrition = Yes)</t>
   </si>
+  <si>
+    <t>Employees with high OT are leaving</t>
+  </si>
+  <si>
+    <t>Reduce overtime</t>
+  </si>
+  <si>
+    <t>Employees with Job level 1 are leaving and Job level 2 are staying</t>
+  </si>
+  <si>
+    <t>Promote faster for high performers</t>
+  </si>
+  <si>
+    <t>Skip - include in executive report</t>
+  </si>
+  <si>
+    <t>Audience = direct line manager</t>
+  </si>
+  <si>
+    <t>Some factors will be skipped as out of influence of line manager</t>
+  </si>
+  <si>
+    <t>Low income - Bin 1 is likely to leave</t>
+  </si>
+  <si>
+    <t>Single employees are more likely to leave</t>
+  </si>
+  <si>
+    <t>Zero stock option - more likely to leave</t>
+  </si>
+  <si>
+    <t>Tie low total woirking years to training and formation activities</t>
+  </si>
+  <si>
+    <t>Skip - covered by total working years</t>
+  </si>
+  <si>
+    <t>See total working years</t>
+  </si>
+  <si>
+    <t>More time in current role related to lower attrition</t>
+  </si>
+  <si>
+    <t>Certain job roles have higher attrition - need to be monitored more closely</t>
+  </si>
+  <si>
+    <t>See years in current role</t>
+  </si>
+  <si>
+    <t>Skip - covered by years in current role</t>
+  </si>
+  <si>
+    <t>Employees with low environment satisfaction are more likely to leave</t>
+  </si>
+  <si>
+    <t>Improve the workplace environment (address issues quoted ny those with value and low satisfaction)</t>
+  </si>
+  <si>
+    <t>Work life balance Bad - more likely to leave</t>
+  </si>
+  <si>
+    <t>Improve worklife balance</t>
+  </si>
+  <si>
+    <t>Recduce business travel where possible</t>
+  </si>
+  <si>
+    <t>More business travel - more likely to leave than if have less business travel</t>
+  </si>
+  <si>
+    <t>If Years at company is high, they are more likely to stay. If low they are likely to leave</t>
+  </si>
+  <si>
+    <t>If total working years is high, they are more likely to stay.If low they are likely to leave</t>
+  </si>
+  <si>
+    <t>High Job involvement - likely to stay, If low they are likely to leave</t>
+  </si>
+  <si>
+    <t>Create personal development plan</t>
+  </si>
+  <si>
+    <t>If numbers of companies is very high (bin 4) more likely to leave than if above average (BIN 3)- out of our control</t>
+  </si>
+  <si>
+    <t>Low Job satisfaction - more likely to leave / High  Job satisfaction more likely to stay</t>
+  </si>
+  <si>
+    <t>Low: create personal development plan, High: Suggest take on mentorship role</t>
+  </si>
+  <si>
+    <t>Sales - more likely to leave / R&amp;D mnore likely to stay</t>
+  </si>
+  <si>
+    <t>Educational field - technical degree slightly more likely to leave. More education might help to retain</t>
+  </si>
+  <si>
+    <t>Bin 1 - more likely to leave</t>
+  </si>
+  <si>
+    <t>High distance from home - more likely to leave</t>
+  </si>
+  <si>
+    <t>Monitor worklife balance</t>
+  </si>
+  <si>
+    <t>Work life</t>
+  </si>
+  <si>
+    <t>Professional development</t>
+  </si>
+  <si>
+    <t>Professional development / Personal development</t>
+  </si>
+  <si>
+    <t>Tie promotion if low to advance faster / Mentor if years at company low</t>
+  </si>
+  <si>
+    <t>Personal development</t>
+  </si>
+  <si>
+    <t>Filtered out skipped strategies</t>
+  </si>
+  <si>
+    <t>Incentivise specialisation or promote  / Mentorships role</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +307,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,12 +337,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,7 +445,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B6:E27" totalsRowShown="0">
-  <autoFilter ref="B6:E27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="B6:E27" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Personal development"/>
+        <filter val="Professional development / Personal development"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Discussion (Hypothesis)"/>
@@ -587,26 +730,32 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="84.140625" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="7" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84.1640625" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="7" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -615,7 +764,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
@@ -623,9 +772,12 @@
         <v>24</v>
       </c>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -639,112 +791,271 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
@@ -752,7 +1063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>